<commit_message>
Fix .gitignore and delete not required files
</commit_message>
<xml_diff>
--- a/功能菜单.xlsx
+++ b/功能菜单.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Files\Project_File\Program_Project\BotScript\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Files\Project_File\Program_Project\BotScript\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774347F1-B73E-4CDE-9DA8-2D30F89D6D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F9B7BD-B69B-4024-A948-DBBE243A4984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="27045" windowHeight="16440" xr2:uid="{CD33FC41-4881-4B3F-A1F3-BF8786641A1A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>指令</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -606,6 +606,46 @@
       </rPr>
       <t>(未实装)</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GitHub仓库地址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/Ginsakura/QQbot_Python</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最新版本号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.0.4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.0.0 Pre</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.4.3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.0.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.1.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.0.3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.0.1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -613,7 +653,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -767,6 +807,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="霞鹜文楷等宽"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF00B0F0"/>
       <name val="霞鹜文楷等宽"/>
       <family val="3"/>
       <charset val="134"/>
@@ -804,7 +852,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -833,8 +881,121 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thick">
         <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color rgb="FF00B0F0"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color rgb="FF00B0F0"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color rgb="FF00B0F0"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color rgb="FF00B0F0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color rgb="FF00B0F0"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color rgb="FF00B0F0"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color rgb="FF00B0F0"/>
       </left>
       <right/>
       <top style="thick">
@@ -846,9 +1007,11 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="dashed">
+        <color rgb="FF00B0F0"/>
+      </left>
       <right/>
-      <top style="thick">
+      <top style="double">
         <color indexed="64"/>
       </top>
       <bottom style="double">
@@ -857,21 +1020,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="dashed">
+        <color rgb="FFC00000"/>
+      </left>
       <right style="thick">
         <color indexed="64"/>
       </right>
-      <top style="thick">
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color rgb="FF00B0F0"/>
+      </left>
+      <right/>
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="double">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color indexed="64"/>
+      <left style="dashed">
+        <color rgb="FF00B0F0"/>
       </left>
       <right/>
       <top/>
@@ -879,8 +1053,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thick">
+      <left style="dashed">
+        <color rgb="FF00B0F0"/>
+      </left>
+      <right style="double">
         <color indexed="64"/>
       </right>
       <top/>
@@ -888,8 +1064,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color indexed="64"/>
+      <left style="dashed">
+        <color rgb="FF00B0F0"/>
       </left>
       <right/>
       <top/>
@@ -899,7 +1075,22 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="dashed">
+        <color rgb="FFC00000"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color rgb="FFC00000"/>
+      </left>
       <right style="thick">
         <color indexed="64"/>
       </right>
@@ -910,10 +1101,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color indexed="64"/>
+      <left style="dashed">
+        <color rgb="FFC00000"/>
       </left>
-      <right/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -923,42 +1116,28 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="dashed">
+        <color rgb="FFC00000"/>
+      </left>
       <right style="thick">
         <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="double">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color rgb="FFC00000"/>
+      </left>
+      <right style="thick">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
       <bottom style="double">
         <color indexed="64"/>
       </bottom>
@@ -973,7 +1152,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -983,128 +1162,134 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1421,299 +1606,346 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{971FCAAC-40A8-4EE5-9F75-39877D21B3CC}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.25" style="32" customWidth="1"/>
-    <col min="2" max="2" width="38" style="11" customWidth="1"/>
-    <col min="3" max="3" width="12.25" style="11" customWidth="1"/>
-    <col min="4" max="4" width="10.25" style="11" customWidth="1"/>
-    <col min="5" max="5" width="11" style="11" customWidth="1"/>
-    <col min="6" max="6" width="12.375" style="11" customWidth="1"/>
-    <col min="7" max="7" width="9" style="8"/>
-    <col min="8" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="17.25" style="19" customWidth="1"/>
+    <col min="2" max="2" width="38" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.25" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.25" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9" style="15"/>
+    <col min="8" max="8" width="16.5" style="42" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:9" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="6"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="40" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:9" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="15"/>
+    </row>
+    <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="13"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="41" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="14" t="s">
+    <row r="4" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="13"/>
+      <c r="G4" s="28"/>
     </row>
-    <row r="4" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="14" t="s">
+    <row r="5" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="13"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="28"/>
     </row>
-    <row r="5" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="14" t="s">
+    <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="13"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="28"/>
     </row>
-    <row r="6" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="14" t="s">
+    <row r="7" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="13"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="28"/>
     </row>
-    <row r="7" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="14" t="s">
+    <row r="8" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="13"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="28"/>
     </row>
-    <row r="8" spans="1:7" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="33"/>
-      <c r="B8" s="15" t="s">
+    <row r="9" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="20"/>
+      <c r="B9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="17"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="43"/>
     </row>
-    <row r="9" spans="1:7" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+    <row r="10" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B10" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C10" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="23"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="44" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="10" spans="1:7" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+    <row r="11" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B11" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C11" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="26"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="42" t="s">
+        <v>58</v>
+      </c>
     </row>
-    <row r="11" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+    <row r="12" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B12" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="13"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="45" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="12" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="29" t="s">
+    <row r="13" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C13" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="28"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
     </row>
-    <row r="13" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="30" t="s">
+    <row r="14" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C14" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19" t="s">
+      <c r="D14" s="34"/>
+      <c r="E14" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="19"/>
-      <c r="G13" s="20"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
     </row>
-    <row r="14" spans="1:7" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="31" t="s">
+    <row r="15" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C15" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="39"/>
-      <c r="E14" s="37" t="s">
+      <c r="D15" s="7"/>
+      <c r="E15" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="37"/>
-      <c r="G14" s="38"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
     </row>
-    <row r="15" spans="1:7" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="33"/>
-      <c r="B15" s="21" t="s">
+    <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="20"/>
+      <c r="B16" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="36"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
     </row>
-    <row r="16" spans="1:7" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+    <row r="17" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B17" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="35"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="45" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="17" spans="1:7" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="40" t="s">
+    <row r="18" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="41" t="s">
+      <c r="B18" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="10"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="45" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="18" spans="1:7" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="40" t="s">
+    <row r="19" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="42" t="s">
+      <c r="B19" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="43"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="45" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H20" s="45"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="C9:G9"/>
+  <mergeCells count="11">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="B17:G17"/>
     <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C14:D14"/>
     <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C10" r:id="rId1" xr:uid="{D02A898C-58F8-4E9D-8B85-1C6F033CC295}"/>
+    <hyperlink ref="C11" r:id="rId1" xr:uid="{D02A898C-58F8-4E9D-8B85-1C6F033CC295}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{32DD36A7-6180-4546-84D7-8604187021E6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix some print problem
</commit_message>
<xml_diff>
--- a/功能菜单.xlsx
+++ b/功能菜单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Files\Project_File\Program_Project\BotScript\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC0DC3F9-5644-49DA-AB7D-2A070EFF33FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F70FF4-4B3C-4D9D-8445-6432D59CF2BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1440" windowWidth="20145" windowHeight="11835" xr2:uid="{CD33FC41-4881-4B3F-A1F3-BF8786641A1A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27090" windowHeight="16440" xr2:uid="{CD33FC41-4881-4B3F-A1F3-BF8786641A1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="68">
   <si>
     <t>指令</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -659,6 +659,13 @@
   <si>
     <t>0.0.1 Pre</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bili视频链接解析</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.0.1 Pre</t>
   </si>
 </sst>
 </file>
@@ -1612,15 +1619,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{971FCAAC-40A8-4EE5-9F75-39877D21B3CC}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H22"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.25" style="11" customWidth="1"/>
+    <col min="1" max="1" width="19.25" style="11" customWidth="1"/>
     <col min="2" max="2" width="38" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.25" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.25" style="1" customWidth="1"/>
@@ -1960,6 +1967,20 @@
       <c r="G21" s="2"/>
       <c r="H21" s="26" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="21"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="26" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>